<commit_message>
data sample and code updated
</commit_message>
<xml_diff>
--- a/my_data/raw_data/labeling_details.xlsx
+++ b/my_data/raw_data/labeling_details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\I3T\Projects\CPR\code base\AR_CPR_SA\my_data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CCA786-AF33-4FBB-8B40-2B04BD5F2B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30539E5E-3035-42D0-AE3F-46292E070DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="28800" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>User</t>
   </si>
@@ -115,9 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,7 +402,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="A4" sqref="A4:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +438,7 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
@@ -466,7 +467,7 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>1</v>
       </c>
     </row>
@@ -489,101 +490,21 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
+      <c r="G7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>